<commit_message>
Created StatisticsRecorder project for save ga statistics to excel file.
</commit_message>
<xml_diff>
--- a/GAExamSchedule/ScheduleData/Ders Eşleştirmeleri.xlsx
+++ b/GAExamSchedule/ScheduleData/Ders Eşleştirmeleri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcht6\source\repos\GAExamSchedule\GAExamSchedule\ScheduleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB971536-EE22-4C64-9B1D-69B62EB92FEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80EEEBE-02B0-4B1B-AAE5-B9D3EF7476F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Zorluk</t>
+  </si>
+  <si>
+    <t>Sınıf Sayısı</t>
   </si>
 </sst>
 </file>
@@ -107,12 +110,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01E95F90-8495-4C20-B6D7-669D33C6CB28}" name="Tablo1" displayName="Tablo1" ref="A1:H29" totalsRowShown="0">
-  <autoFilter ref="A1:H29" xr:uid="{97CFA720-D15B-4545-9496-9AAF040BF23F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01E95F90-8495-4C20-B6D7-669D33C6CB28}" name="Tablo1" displayName="Tablo1" ref="A1:I29" totalsRowShown="0">
+  <autoFilter ref="A1:I29" xr:uid="{97CFA720-D15B-4545-9496-9AAF040BF23F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
     <sortCondition ref="A1:A17"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BA756C68-461A-4DE7-8F9B-C5D17F55712D}" name="ID"/>
     <tableColumn id="2" xr3:uid="{F92667C9-B76B-4CC8-A151-8A07A1483D51}" name="Ders"/>
     <tableColumn id="3" xr3:uid="{4E99577D-0171-40E1-83D8-AC4C0E25D1CA}" name="Öğretim Görevlisi"/>
@@ -121,6 +124,7 @@
     <tableColumn id="6" xr3:uid="{CD6186F9-608C-41C9-93CC-741E77862B4F}" name="Laboratuvar Gereksinimi (E - H)"/>
     <tableColumn id="7" xr3:uid="{1B634FA2-8C2F-40A9-B561-63620074B0D4}" name="Öğrenci Sayısı"/>
     <tableColumn id="8" xr3:uid="{6FCE4EE1-7A26-4B09-89C4-5BD6B2EE2368}" name="Zorluk"/>
+    <tableColumn id="9" xr3:uid="{04857D93-366D-4A91-9EC7-7235D31969AE}" name="Sınıf Sayısı"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -389,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +409,7 @@
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,8 +434,11 @@
       <c r="H1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -456,8 +463,11 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -482,8 +492,11 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -508,8 +521,11 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -534,8 +550,11 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -560,8 +579,11 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -586,8 +608,11 @@
       <c r="H7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -612,8 +637,11 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -638,8 +666,11 @@
       <c r="H9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -664,8 +695,11 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -690,8 +724,11 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -716,8 +753,11 @@
       <c r="H12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -742,8 +782,11 @@
       <c r="H13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -768,8 +811,11 @@
       <c r="H14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -794,8 +840,11 @@
       <c r="H15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -820,8 +869,11 @@
       <c r="H16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -846,8 +898,11 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -872,8 +927,11 @@
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -898,8 +956,11 @@
       <c r="H19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -924,8 +985,11 @@
       <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -950,8 +1014,11 @@
       <c r="H21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -976,8 +1043,11 @@
       <c r="H22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1002,8 +1072,11 @@
       <c r="H23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1028,8 +1101,11 @@
       <c r="H24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1054,8 +1130,11 @@
       <c r="H25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1080,8 +1159,11 @@
       <c r="H26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1106,8 +1188,11 @@
       <c r="H27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1132,8 +1217,11 @@
       <c r="H28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1157,6 +1245,9 @@
       </c>
       <c r="H29">
         <v>2</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed course classes count calculate.
</commit_message>
<xml_diff>
--- a/GAExamSchedule/ScheduleData/Ders Eşleştirmeleri.xlsx
+++ b/GAExamSchedule/ScheduleData/Ders Eşleştirmeleri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcht6\source\repos\GAExamSchedule\GAExamSchedule\ScheduleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80EEEBE-02B0-4B1B-AAE5-B9D3EF7476F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9AD126-3496-4DFD-8157-0294D78E38A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="I2" sqref="I2:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,6 +407,7 @@
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -464,7 +465,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -493,7 +494,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -522,7 +523,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -551,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -580,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -609,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -638,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -667,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -696,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -725,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -754,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -783,7 +784,7 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -812,7 +813,7 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -841,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -870,7 +871,7 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -899,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -928,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -957,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -986,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1015,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1044,7 +1045,7 @@
         <v>2</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1073,7 +1074,7 @@
         <v>2</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1102,7 +1103,7 @@
         <v>3</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1131,7 +1132,7 @@
         <v>1</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,7 +1161,7 @@
         <v>3</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1189,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1218,7 +1219,7 @@
         <v>3</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1247,7 +1248,7 @@
         <v>2</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GA parameters config applied to algorithm.
</commit_message>
<xml_diff>
--- a/GAExamSchedule/ScheduleData/Ders Eşleştirmeleri.xlsx
+++ b/GAExamSchedule/ScheduleData/Ders Eşleştirmeleri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcht6\source\repos\GAExamSchedule\GAExamSchedule\ScheduleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9AD126-3496-4DFD-8157-0294D78E38A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593363B8-7857-42FF-BC00-A1D87FA366F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
   <si>
     <t>Öğrenci Sayısı</t>
   </si>
@@ -110,13 +107,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01E95F90-8495-4C20-B6D7-669D33C6CB28}" name="Tablo1" displayName="Tablo1" ref="A1:I29" totalsRowShown="0">
-  <autoFilter ref="A1:I29" xr:uid="{97CFA720-D15B-4545-9496-9AAF040BF23F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
-    <sortCondition ref="A1:A17"/>
-  </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{BA756C68-461A-4DE7-8F9B-C5D17F55712D}" name="ID"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01E95F90-8495-4C20-B6D7-669D33C6CB28}" name="Tablo1" displayName="Tablo1" ref="A1:H29" totalsRowShown="0">
+  <autoFilter ref="A1:H29" xr:uid="{97CFA720-D15B-4545-9496-9AAF040BF23F}"/>
+  <tableColumns count="8">
     <tableColumn id="2" xr3:uid="{F92667C9-B76B-4CC8-A151-8A07A1483D51}" name="Ders"/>
     <tableColumn id="3" xr3:uid="{4E99577D-0171-40E1-83D8-AC4C0E25D1CA}" name="Öğretim Görevlisi"/>
     <tableColumn id="4" xr3:uid="{CF1CBA5F-007E-48CD-922B-3B6F9EEFDB6D}" name="Süre"/>
@@ -393,26 +386,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I29"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -427,19 +420,16 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -447,144 +437,129 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
       </c>
       <c r="G2">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
       </c>
       <c r="G3">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
       </c>
       <c r="G4">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
       </c>
       <c r="G5">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -592,662 +567,593 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>40</v>
       </c>
       <c r="G7">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
       </c>
       <c r="G8">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>40</v>
       </c>
       <c r="G9">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>40</v>
       </c>
       <c r="G10">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
-        <v>7</v>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
       </c>
       <c r="G11">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
-        <v>7</v>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>40</v>
       </c>
       <c r="G12">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
         <v>3</v>
       </c>
-      <c r="F13" t="s">
-        <v>7</v>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
       </c>
       <c r="G13">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
-        <v>7</v>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>40</v>
       </c>
       <c r="G14">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
         <v>4</v>
       </c>
-      <c r="F15" t="s">
-        <v>7</v>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
       </c>
       <c r="G15">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
         <v>4</v>
       </c>
-      <c r="F16" t="s">
-        <v>7</v>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>40</v>
       </c>
       <c r="G16">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
         <v>4</v>
       </c>
-      <c r="F17" t="s">
-        <v>7</v>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>40</v>
       </c>
       <c r="G17">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
         <v>5</v>
       </c>
-      <c r="F18" t="s">
-        <v>7</v>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>40</v>
       </c>
       <c r="G18">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C19">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
         <v>5</v>
       </c>
-      <c r="F19" t="s">
-        <v>7</v>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>40</v>
       </c>
       <c r="G19">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C20">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>40</v>
       </c>
       <c r="G20">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>40</v>
       </c>
       <c r="G21">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <v>2</v>
       </c>
-      <c r="I21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>6</v>
-      </c>
-      <c r="F22" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>40</v>
       </c>
       <c r="G22">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>2</v>
       </c>
-      <c r="I22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
         <v>7</v>
       </c>
-      <c r="F23" t="s">
-        <v>7</v>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23">
+        <v>40</v>
       </c>
       <c r="G23">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>2</v>
       </c>
-      <c r="I23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
         <v>7</v>
       </c>
-      <c r="F24" t="s">
-        <v>7</v>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>40</v>
       </c>
       <c r="G24">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="H24">
-        <v>3</v>
-      </c>
-      <c r="I24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25">
         <v>7</v>
       </c>
-      <c r="F25" t="s">
-        <v>7</v>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>40</v>
       </c>
       <c r="G25">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
         <v>8</v>
       </c>
-      <c r="F26" t="s">
-        <v>7</v>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26">
+        <v>40</v>
       </c>
       <c r="G26">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="H26">
-        <v>3</v>
-      </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>2</v>
-      </c>
-      <c r="E27">
         <v>8</v>
       </c>
-      <c r="F27" t="s">
-        <v>7</v>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>40</v>
       </c>
       <c r="G27">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H27">
         <v>2</v>
       </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28">
         <v>8</v>
       </c>
-      <c r="F28" t="s">
-        <v>7</v>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>40</v>
       </c>
       <c r="G28">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="H28">
-        <v>3</v>
-      </c>
-      <c r="I28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C29">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="E29">
         <v>8</v>
       </c>
-      <c r="F29" t="s">
-        <v>7</v>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29">
+        <v>40</v>
       </c>
       <c r="G29">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H29">
-        <v>2</v>
-      </c>
-      <c r="I29">
         <v>2</v>
       </c>
     </row>

</xml_diff>